<commit_message>
Auto stash before rebase of "refs/heads/main"
</commit_message>
<xml_diff>
--- a/consolidacao/CJBG_consolidacao.xlsx
+++ b/consolidacao/CJBG_consolidacao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I230"/>
+  <dimension ref="A1:I228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1400,7 +1400,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1929,7 +1929,7 @@
         </is>
       </c>
       <c r="G35" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -2875,7 +2875,7 @@
         </is>
       </c>
       <c r="G57" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -3335,7 +3335,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -3864,7 +3864,7 @@
         </is>
       </c>
       <c r="G80" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
@@ -5750,12 +5750,22 @@
           <t>17 - MATERIAL DE PROCESSAMENTO DE DADOS</t>
         </is>
       </c>
-      <c r="F124" t="inlineStr"/>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>CABO ÁUDIO E VÍDEO, APLICAÇÃO PARA DATASHOW, TIPO CABO VGA, QUANTIDADE DE VIAS15 .</t>
+        </is>
+      </c>
+      <c r="G124" t="n">
+        <v>21</v>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+        </is>
+      </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>left_only</t>
+          <t>both</t>
         </is>
       </c>
     </row>
@@ -5776,7 +5786,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -6292,7 +6302,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -7066,7 +7076,7 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -7224,21 +7234,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>30.22.752</t>
+          <t>30.22.753</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>DILUIDOR DE PRODUTO QUÍMICO, EQUIPAMENTO PARA SERVIÇOS DIVERSOS PROFISSIONAIS, PADRÃO MANUAL, MATERIAL METAL PLÁSTICO.</t>
+          <t>ÁLCOOL ETÍLICO, TIPO HIDRATADO, TEOR ALCOÓLICA 70 (70° GL), COMPOSIÇÃO BÁSICA COM CARBOCOL E GLICERINA, CARACTERÍSTICAS ADICIONAIS BAG IN BOX, COM BICO DOSADOR, REFIL</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -7246,23 +7256,29 @@
         </is>
       </c>
       <c r="F159" t="inlineStr"/>
-      <c r="G159" t="inlineStr"/>
-      <c r="H159" t="inlineStr"/>
+      <c r="G159" t="n">
+        <v>22</v>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+        </is>
+      </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>left_only</t>
+          <t>both</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>30.22.753</t>
+          <t>30.22.754</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>ÁLCOOL ETÍLICO, TIPO HIDRATADO, TEOR ALCOÓLICA 70 (70° GL), COMPOSIÇÃO BÁSICA COM CARBOCOL E GLICERINA, CARACTERÍSTICAS ADICIONAIS BAG IN BOX, COM BICO DOSADOR, REFIL</t>
+          <t>DESINFETANTE, COMPOSIÇÃO A BASE DE QUATERNÁRIO DE AMÔNIA, PRINCIPIO ATIVO CLORETO ALQUIL DIMETIL BENZIL AMÔNIA + TENCIOATIVO S, TEOR ATIVO EM TORNO DE 1,5, FORMA FÍSICA SOLUÇÃO AQUOSA. GALÃO 5 LITROS.</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -7271,16 +7287,20 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
           <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
         </is>
       </c>
-      <c r="F160" t="inlineStr"/>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>DESINFETANTE, COMPOSI</t>
+        </is>
+      </c>
       <c r="G160" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="H160" t="inlineStr">
         <is>
@@ -7296,21 +7316,21 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>30.22.754</t>
+          <t>30.22.755</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>DESINFETANTE, COMPOSIÇÃO A BASE DE QUATERNÁRIO DE AMÔNIA, PRINCIPIO ATIVO CLORETO ALQUIL DIMETIL BENZIL AMÔNIA + TENCIOATIVO S, TEOR ATIVO EM TORNO DE 1,5, FORMA FÍSICA SOLUÇÃO AQUOSA. GALÃO 5 LITROS.</t>
+          <t>PANO DE LIMPEZA,MATERIAL 100 ALGODÃO, COMPRIMENTO 70 CM, LARGURA 50 CM, CARACTERÍSTICAS ADICIONAL COR BRANCA</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -7319,11 +7339,11 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>DESINFETANTE, COMPOSI</t>
+          <t>PANO DE LIMPEZA,MATERIAL 100 ALGOD</t>
         </is>
       </c>
       <c r="G161" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="H161" t="inlineStr">
         <is>
@@ -7339,34 +7359,30 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>30.22.755</t>
+          <t>30.22.756</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>PANO DE LIMPEZA,MATERIAL 100 ALGODÃO, COMPRIMENTO 70 CM, LARGURA 50 CM, CARACTERÍSTICAS ADICIONAL COR BRANCA</t>
+          <t>ÁLCOOL ETÍLICO HIDRATADO, APRESENTAÇÃO GEL, CONCENTRAÇÃO 70º</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
           <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
         </is>
       </c>
-      <c r="F162" t="inlineStr">
-        <is>
-          <t>PANO DE LIMPEZA,MATERIAL 100 ALGOD</t>
-        </is>
-      </c>
+      <c r="F162" t="inlineStr"/>
       <c r="G162" t="n">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="H162" t="inlineStr">
         <is>
@@ -7382,30 +7398,34 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>30.22.756</t>
+          <t>30.22.757</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>ÁLCOOL ETÍLICO HIDRATADO, APRESENTAÇÃO GEL, CONCENTRAÇÃO 70º</t>
+          <t>SABONETEIRA, MATERIAL SUPORTE PLÁSTICO ABS, MATERIAL RESERVATÓRIO PLÁSTICO ABS, ACABAMENTO SUPERFICIAL SUPORTE PLÁSTICO,ALTURA 23 CM, LARGURA 11 CM,, CAPACIDADE 1000ML, FIXAÇÃO EM PAREDE COM BUCHA, PARAFUSO TIPO USO DOMESTICO, COM USO DO REFIL.</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
           <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
         </is>
       </c>
-      <c r="F163" t="inlineStr"/>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>SABONETEIRA, MATERIAL SUPORTE PL</t>
+        </is>
+      </c>
       <c r="G163" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="H163" t="inlineStr">
         <is>
@@ -7421,12 +7441,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>30.22.757</t>
+          <t>30.22.758</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>SABONETEIRA, MATERIAL SUPORTE PLÁSTICO ABS, MATERIAL RESERVATÓRIO PLÁSTICO ABS, ACABAMENTO SUPERFICIAL SUPORTE PLÁSTICO,ALTURA 23 CM, LARGURA 11 CM,, CAPACIDADE 1000ML, FIXAÇÃO EM PAREDE COM BUCHA, PARAFUSO TIPO USO DOMESTICO, COM USO DO REFIL.</t>
+          <t>SABONETE LIQUIDO ASPECTO FÍSICO LIQUIDO VISCOSO, ACIDEZ PH 6 A 8,APLICAÇÃO ASSEPSIA DAS MÃOS , COMPOSIÇÃO TENSOATIVOS ANIÔNICO E NÃO ANIÔNICO, SOLVENTE</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -7435,7 +7455,7 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -7444,11 +7464,11 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>SABONETEIRA, MATERIAL SUPORTE PL</t>
+          <t>SABONETE LIQUIDO ASPECTO F</t>
         </is>
       </c>
       <c r="G164" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H164" t="inlineStr">
         <is>
@@ -7464,12 +7484,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>30.22.758</t>
+          <t>30.22.759</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>SABONETE LIQUIDO ASPECTO FÍSICO LIQUIDO VISCOSO, ACIDEZ PH 6 A 8,APLICAÇÃO ASSEPSIA DAS MÃOS , COMPOSIÇÃO TENSOATIVOS ANIÔNICO E NÃO ANIÔNICO, SOLVENTE</t>
+          <t>SABONETEIRA, ALTURA 28,70 CM, LARGURA 12, 50 CM, CAPACIDADE 800 ML, TIPO FIXAÇÃO EM PAREDE ATRAVÉS DE BUCHA E PARAFUSO,TIPO USO REFIL 800 ML, TIPO BAG IN BOX,SISTEMA DE TRAVAS LATERAL ACIONADA POR PRESSÃO.</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -7478,7 +7498,7 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -7487,11 +7507,11 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>SABONETE LIQUIDO ASPECTO F</t>
+          <t>SABONETEIRA, ALTURA 28,70 CM, LARGURA 12, 50 CM, CAPACIDADE 800 ML, TIPO FIXA</t>
         </is>
       </c>
       <c r="G165" t="n">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="H165" t="inlineStr">
         <is>
@@ -7507,12 +7527,12 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>30.22.759</t>
+          <t>30.22.80</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>SABONETEIRA, ALTURA 28,70 CM, LARGURA 12, 50 CM, CAPACIDADE 800 ML, TIPO FIXAÇÃO EM PAREDE ATRAVÉS DE BUCHA E PARAFUSO,TIPO USO REFIL 800 ML, TIPO BAG IN BOX,SISTEMA DE TRAVAS LATERAL ACIONADA POR PRESSÃO.</t>
+          <t>BALDE PLÁSTICO COM ALÇA 20 L.</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -7521,7 +7541,7 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -7530,11 +7550,11 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>SABONETEIRA, ALTURA 28,70 CM, LARGURA 12, 50 CM, CAPACIDADE 800 ML, TIPO FIXA</t>
+          <t>BALDE PL</t>
         </is>
       </c>
       <c r="G166" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="H166" t="inlineStr">
         <is>
@@ -7550,12 +7570,12 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>30.22.80</t>
+          <t>30.22.802</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>BALDE PLÁSTICO COM ALÇA 20 L.</t>
+          <t>FILME PLÁSTICO, TIPO ESTIRÁVEL, LARGURA 10 CM, APLICAÇÃO EMBALAR VIDRARIAS, MATERIAL PVC, COMPRIMENTO 38 M</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -7564,7 +7584,7 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -7573,11 +7593,11 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>BALDE PL</t>
+          <t>FILME PL</t>
         </is>
       </c>
       <c r="G167" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
@@ -7593,21 +7613,21 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>30.22.802</t>
+          <t>30.22.805</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>FILME PLÁSTICO, TIPO ESTIRÁVEL, LARGURA 10 CM, APLICAÇÃO EMBALAR VIDRARIAS, MATERIAL PVC, COMPRIMENTO 38 M</t>
+          <t>VESTUÁRIO DE PROTEÇÃO, AVENTAL DESCARTÁVEL, GRAMATURA 30/M², MANGA LONGA COM PUNHO.</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>Conjunto</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -7616,15 +7636,15 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>FILME PL</t>
+          <t>VESTUÁRIO DE PROTEÇÃO, AVENTAL DESCARTÁVEL, GRAMATURA 30/M², MANGA LONGA COM PUNHO.</t>
         </is>
       </c>
       <c r="G168" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
@@ -7636,21 +7656,21 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>30.22.805</t>
+          <t>30.22.806</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>VESTUÁRIO DE PROTEÇÃO, AVENTAL DESCARTÁVEL, GRAMATURA 30/M², MANGA LONGA COM PUNHO.</t>
+          <t>TAPETE, MATERIAL SUPERFÍCIE VINIL, BASE PVC, TIPO BORRACHA ANTIDERRAPANTE, 38 CM X 158 CM, COR PRETA, SANITIZANTE,</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Conjunto</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -7659,15 +7679,15 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>VESTUÁRIO DE PROTEÇÃO, AVENTAL DESCARTÁVEL, GRAMATURA 30/M², MANGA LONGA COM PUNHO.</t>
+          <t>TAPETE, MATERIAL SUPERF</t>
         </is>
       </c>
       <c r="G169" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
@@ -7679,12 +7699,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>30.22.806</t>
+          <t>30.22.807</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>TAPETE, MATERIAL SUPERFÍCIE VINIL, BASE PVC, TIPO BORRACHA ANTIDERRAPANTE, 38 CM X 158 CM, COR PRETA, SANITIZANTE,</t>
+          <t>Fita adesiva, cor vermelha, material polipropileno, 20mm x 30m</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -7693,7 +7713,7 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -7702,15 +7722,15 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>TAPETE, MATERIAL SUPERF</t>
+          <t>Fita adesiva, cor vermelha, material polipropileno, 20mm x 30m</t>
         </is>
       </c>
       <c r="G170" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -7722,12 +7742,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>30.22.807</t>
+          <t>30.22.808</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Fita adesiva, cor vermelha, material polipropileno, 20mm x 30m</t>
+          <t>Termômetro clínico, digital, infravermelho, uso em testa, escala até 50º C, memória até 10 medições.</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -7736,7 +7756,7 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -7745,15 +7765,15 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Fita adesiva, cor vermelha, material polipropileno, 20mm x 30m</t>
+          <t>Term</t>
         </is>
       </c>
       <c r="G171" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
@@ -7765,12 +7785,12 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>30.22.808</t>
+          <t>30.23.755</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Termômetro clínico, digital, infravermelho, uso em testa, escala até 50º C, memória até 10 medições.</t>
+          <t>FAIXA PARA CINTURA AJUSTÁVEL EM CETIM, COM VELCRO, ENTRE 8 E 10CM DE LARGURA E 1,10 E 1,50M DE COMPRIMENTO</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -7779,20 +7799,20 @@
         </is>
       </c>
       <c r="D172" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
+          <t>23 - UNIFORMES, TECIDOS E AVIAMENTOS</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>Term</t>
+          <t>FAIXA PARA CINTURA AJUST</t>
         </is>
       </c>
       <c r="G172" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="H172" t="inlineStr">
         <is>
@@ -7808,12 +7828,12 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>30.23.755</t>
+          <t>30.23.817</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>FAIXA PARA CINTURA AJUSTÁVEL EM CETIM, COM VELCRO, ENTRE 8 E 10CM DE LARGURA E 1,10 E 1,50M DE COMPRIMENTO</t>
+          <t>TOGA, MATERIAL CETIM, COR PRETA, APLICAÇÃO SOLENIDADES</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -7822,7 +7842,7 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -7831,11 +7851,11 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>FAIXA PARA CINTURA AJUST</t>
+          <t>TOGA, MATERIAL CETIM, COR PRETA, APLICA</t>
         </is>
       </c>
       <c r="G173" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H173" t="inlineStr">
         <is>
@@ -7851,12 +7871,12 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>30.23.817</t>
+          <t>30.23.818</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>TOGA, MATERIAL CETIM, COR PRETA, APLICAÇÃO SOLENIDADES</t>
+          <t>CHAPÉU MASCULINO, CAPELO AJUSTÁVEL, CONFECCIONADO EM TECIDO OXFORD PRETO, AJUSTÁVEL EM VELCRO.</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -7874,11 +7894,11 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>TOGA, MATERIAL CETIM, COR PRETA, APLICA</t>
+          <t>CHAP</t>
         </is>
       </c>
       <c r="G174" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H174" t="inlineStr">
         <is>
@@ -7894,12 +7914,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>30.23.818</t>
+          <t>30.24.1065</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>CHAPÉU MASCULINO, CAPELO AJUSTÁVEL, CONFECCIONADO EM TECIDO OXFORD PRETO, AJUSTÁVEL EM VELCRO.</t>
+          <t>ROLO PINTURA PREDIAL, LÃ DE CARNEIRO, TUBO PLÁSTICO, APLICAÇÃO SUPERFÍCIE LISA/LÁTEX E ACRÍLICA, COMPRIMENTO 9 CM, CABO PLÁSTICO RESISTENTE</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -7908,24 +7928,24 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>23 - UNIFORMES, TECIDOS E AVIAMENTOS</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>CHAP</t>
+          <t>ROLO PINTURA PREDIAL, LÃ DE CARNEIRO, TUBO PLÁSTICO, APLICAÇÃO SUPERFÍCIE LISA/LÁTEX E ACRÍLICA, COMPRIMENTO 9 CM, CABO PLÁSTICO RESISTENTE</t>
         </is>
       </c>
       <c r="G175" t="n">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
@@ -7937,12 +7957,12 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>30.24.1065</t>
+          <t>30.24.1338</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>ROLO PINTURA PREDIAL, LÃ DE CARNEIRO, TUBO PLÁSTICO, APLICAÇÃO SUPERFÍCIE LISA/LÁTEX E ACRÍLICA, COMPRIMENTO 9 CM, CABO PLÁSTICO RESISTENTE</t>
+          <t>BUCHA PARA PARAFUSO, EM NYLON Nº8.</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -7951,7 +7971,7 @@
         </is>
       </c>
       <c r="D176" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -7960,15 +7980,15 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>ROLO PINTURA PREDIAL, LÃ DE CARNEIRO, TUBO PLÁSTICO, APLICAÇÃO SUPERFÍCIE LISA/LÁTEX E ACRÍLICA, COMPRIMENTO 9 CM, CABO PLÁSTICO RESISTENTE</t>
+          <t>BUCHA PARA PARAFUSO, EM NYLON N</t>
         </is>
       </c>
       <c r="G176" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
@@ -7980,12 +8000,12 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>30.24.1338</t>
+          <t>30.24.1669</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>BUCHA PARA PARAFUSO, EM NYLON Nº8.</t>
+          <t>ADESIVO CONEXÃO HIDRÁULICA, COMPOSIÇÃO BISNAGAS DUPLAS PARA MISTURA INSTANTÂNEA, APLICAÇÃO TUBOS E CONEXÕES DE PVC, COLAGEM ULTRA RÁPIDA, FRASCO COM 175 G</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -7994,7 +8014,7 @@
         </is>
       </c>
       <c r="D177" t="n">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -8003,15 +8023,15 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>BUCHA PARA PARAFUSO, EM NYLON N</t>
+          <t>ADESIVO CONEXÃO HIDRÁULICA, COMPOSIÇÃO BISNAGAS DUPLAS PARA MISTURA INSTANTÂNEA, APLICAÇÃO TUBOS E CONEXÕES DE PVC, COLAGEM ULTRA RÁPIDA, FRASCO COM 175 G</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I177" t="inlineStr">
@@ -8023,12 +8043,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>30.24.1669</t>
+          <t>30.24.1816</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>ADESIVO CONEXÃO HIDRÁULICA, COMPOSIÇÃO BISNAGAS DUPLAS PARA MISTURA INSTANTÂNEA, APLICAÇÃO TUBOS E CONEXÕES DE PVC, COLAGEM ULTRA RÁPIDA, FRASCO COM 175 G</t>
+          <t>FITA VEDA ROSCA 50M X 18MM, ESPESSURA 0,06 A 0,08MM</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -8037,7 +8057,7 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -8046,11 +8066,11 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>ADESIVO CONEXÃO HIDRÁULICA, COMPOSIÇÃO BISNAGAS DUPLAS PARA MISTURA INSTANTÂNEA, APLICAÇÃO TUBOS E CONEXÕES DE PVC, COLAGEM ULTRA RÁPIDA, FRASCO COM 175 G</t>
+          <t>FITA VEDA ROSCA 50M X 18MM, ESPESSURA 0,06 A 0,08MM</t>
         </is>
       </c>
       <c r="G178" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H178" t="inlineStr">
         <is>
@@ -8066,21 +8086,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>30.24.1816</t>
+          <t>30.24.2269</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>FITA VEDA ROSCA 50M X 18MM, ESPESSURA 0,06 A 0,08MM</t>
+          <t>SIFÃO, CONEXÃO HIDRÁULICA PARA USO EM PIA DE LAVATÓRIO</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>PÇ</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -8089,11 +8109,11 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>FITA VEDA ROSCA 50M X 18MM, ESPESSURA 0,06 A 0,08MM</t>
+          <t>SIFÃO, CONEXÃO HIDRÁULICA PARA USO EM PIA DE LAVATÓRIO</t>
         </is>
       </c>
       <c r="G179" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H179" t="inlineStr">
         <is>
@@ -8109,21 +8129,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>30.24.2269</t>
+          <t>30.24.2602</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>SIFÃO, CONEXÃO HIDRÁULICA PARA USO EM PIA DE LAVATÓRIO</t>
+          <t>BÓIA CAIXA D'ÁGUA , BOIA PARA CAIXA D'ÁGUA EM PVC, BITOLA DE 3/4 mARCA: alumasa</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>PÇ</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -8132,11 +8152,11 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>SIFÃO, CONEXÃO HIDRÁULICA PARA USO EM PIA DE LAVATÓRIO</t>
+          <t>BÓIA CAIXA D'ÁGUA , BOIA PARA CAIXA D'ÁGUA EM PVC, BITOLA DE 3/4 mARCA: alumasa</t>
         </is>
       </c>
       <c r="G180" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H180" t="inlineStr">
         <is>
@@ -8152,45 +8172,55 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>30.24.2564</t>
+          <t>30.24.2661</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>PREGO com cabeça de 21/2 x 12</t>
+          <t>BROXA PINTURA ( pincel) de 3</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D181" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
           <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
-      <c r="F181" t="inlineStr"/>
-      <c r="G181" t="inlineStr"/>
-      <c r="H181" t="inlineStr"/>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>BROXA PINTURA ( pincel) de 3</t>
+        </is>
+      </c>
+      <c r="G181" t="n">
+        <v>3</v>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
+        </is>
+      </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>left_only</t>
+          <t>both</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>30.24.2602</t>
+          <t>30.24.2697</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>BÓIA CAIXA D'ÁGUA , BOIA PARA CAIXA D'ÁGUA EM PVC, BITOLA DE 3/4 mARCA: alumasa</t>
+          <t>CONEXÃO HIDRAULICA, MATERIAL PVC- CLORETO DE POLIVINA, TIPO LUVA, TIPO FIXAÇÃO, BITOLA 25</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -8199,7 +8229,7 @@
         </is>
       </c>
       <c r="D182" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -8208,11 +8238,11 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>BÓIA CAIXA D'ÁGUA , BOIA PARA CAIXA D'ÁGUA EM PVC, BITOLA DE 3/4 mARCA: alumasa</t>
+          <t>CONEXÃO HIDRAULICA, MATERIAL PVC- CLORETO DE POLIVINA, TIPO LUVA, TIPO FIXAÇÃO, BITOLA 25</t>
         </is>
       </c>
       <c r="G182" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H182" t="inlineStr">
         <is>
@@ -8228,12 +8258,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>30.24.2661</t>
+          <t>30.24.2711</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>BROXA PINTURA ( pincel) de 3</t>
+          <t>CONEXÃO HIDRAULICA, MATERIAL PVC, TIPO TAMPÃO, TIPO FIXAÇÃO ROSCÁVEL, BITOLA 1/2 POL</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -8242,7 +8272,7 @@
         </is>
       </c>
       <c r="D183" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -8251,11 +8281,11 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>BROXA PINTURA ( pincel) de 3</t>
+          <t>CONEXÃO HIDRAULICA, MATERIAL PVC, TIPO TAMPÃO, TIPO FIXAÇÃO ROSCÁVEL, BITOLA 1/2 POL</t>
         </is>
       </c>
       <c r="G183" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H183" t="inlineStr">
         <is>
@@ -8271,12 +8301,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>30.24.2697</t>
+          <t>30.24.2805</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRAULICA, MATERIAL PVC- CLORETO DE POLIVINA, TIPO LUVA, TIPO FIXAÇÃO, BITOLA 25</t>
+          <t>CONEXÃO HIDRÁULICA, MATERIAL PVC, TIPO TÊ 90º, FIXAÇÃO SOLDÁVEL. APLICAÇÃO PREDIAL ÁGUA FRIA, BITOLA 40 MM.</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -8285,7 +8315,7 @@
         </is>
       </c>
       <c r="D184" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -8294,11 +8324,11 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRAULICA, MATERIAL PVC- CLORETO DE POLIVINA, TIPO LUVA, TIPO FIXAÇÃO, BITOLA 25</t>
+          <t>CONEXÃO HIDRÁULICA, MATERIAL PVC, TIPO TÊ 90º, FIXAÇÃO SOLDÁVEL. APLICAÇÃO PREDIAL ÁGUA FRIA, BITOLA 40 MM.</t>
         </is>
       </c>
       <c r="G184" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H184" t="inlineStr">
         <is>
@@ -8314,12 +8344,12 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>30.24.2711</t>
+          <t>30.24.2814</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRAULICA, MATERIAL PVC, TIPO TAMPÃO, TIPO FIXAÇÃO ROSCÁVEL, BITOLA 1/2 POL</t>
+          <t>CONEXÃO HIDRÁULICA, PVC, TIPO TÊ 90°, ÁGUA FRIA, 25MM</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -8328,7 +8358,7 @@
         </is>
       </c>
       <c r="D185" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -8337,11 +8367,11 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRAULICA, MATERIAL PVC, TIPO TAMPÃO, TIPO FIXAÇÃO ROSCÁVEL, BITOLA 1/2 POL</t>
+          <t>CONEXÃO HIDRÁULICA, PVC, TIPO TÊ 90°, ÁGUA FRIA, 25MM</t>
         </is>
       </c>
       <c r="G185" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H185" t="inlineStr">
         <is>
@@ -8357,12 +8387,12 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>30.24.2805</t>
+          <t>30.24.2819</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRÁULICA, MATERIAL PVC, TIPO TÊ 90º, FIXAÇÃO SOLDÁVEL. APLICAÇÃO PREDIAL ÁGUA FRIA, BITOLA 40 MM.</t>
+          <t>PARAFUSO DE FENDA 8MM</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -8371,7 +8401,7 @@
         </is>
       </c>
       <c r="D186" t="n">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -8380,15 +8410,15 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRÁULICA, MATERIAL PVC, TIPO TÊ 90º, FIXAÇÃO SOLDÁVEL. APLICAÇÃO PREDIAL ÁGUA FRIA, BITOLA 40 MM.</t>
+          <t>PARAFUSO DE FENDA 8MM</t>
         </is>
       </c>
       <c r="G186" t="n">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -8400,21 +8430,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>30.24.2814</t>
+          <t>30.24.2824</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRÁULICA, PVC, TIPO TÊ 90°, ÁGUA FRIA, 25MM</t>
+          <t>PREGO COM CABEÇA DE 11/4 X 14.</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>KG</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -8423,15 +8453,15 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRÁULICA, PVC, TIPO TÊ 90°, ÁGUA FRIA, 25MM</t>
+          <t>PREGO COM CABE</t>
         </is>
       </c>
       <c r="G187" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -8443,12 +8473,12 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>30.24.2819</t>
+          <t>30.24.2858</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>PARAFUSO DE FENDA 8MM</t>
+          <t>MÁSCARA DESCARTÁVEL USO GERAL, POLIPROPILENO, FIXAÇÃO COM CLIPE E ELÁSTICO.</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -8457,7 +8487,7 @@
         </is>
       </c>
       <c r="D188" t="n">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -8466,11 +8496,11 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>PARAFUSO DE FENDA 8MM</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G188" t="n">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="H188" t="inlineStr">
         <is>
@@ -8486,21 +8516,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>30.24.2824</t>
+          <t>30.24.946</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>PREGO COM CABEÇA DE 11/4 X 14.</t>
+          <t>ROLO DE LA DE CARNEIRO, PARA PINTURA DE PAREDES, TAMANHO 23 CM.</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -8509,15 +8539,15 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>PREGO COM CABE</t>
+          <t>ROLO DE LA DE CARNEIRO, PARA PINTURA DE PAREDES, TAMANHO 23 CM.</t>
         </is>
       </c>
       <c r="G189" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
@@ -8529,12 +8559,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>30.24.2858</t>
+          <t>30.24.971</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>MÁSCARA DESCARTÁVEL USO GERAL, POLIPROPILENO, FIXAÇÃO COM CLIPE E ELÁSTICO.</t>
+          <t>TAMPÃO - 1/2 LISO PVC</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -8543,7 +8573,7 @@
         </is>
       </c>
       <c r="D190" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -8552,15 +8582,15 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>TAMPÃO - 1/2 LISO PVC</t>
         </is>
       </c>
       <c r="G190" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
@@ -8572,12 +8602,12 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>30.24.946</t>
+          <t>30.26.1156</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>ROLO DE LA DE CARNEIRO, PARA PINTURA DE PAREDES, TAMANHO 23 CM.</t>
+          <t>Curva 90º para eletroduto PVC rígido, anti-chama, ¾”, fabricante nacional</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -8586,20 +8616,20 @@
         </is>
       </c>
       <c r="D191" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>ROLO DE LA DE CARNEIRO, PARA PINTURA DE PAREDES, TAMANHO 23 CM.</t>
+          <t>Curva 90º para eletroduto PVC rígido, anti-chama, ¾”, fabricante nacional</t>
         </is>
       </c>
       <c r="G191" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H191" t="inlineStr">
         <is>
@@ -8615,12 +8645,12 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>30.24.971</t>
+          <t>30.26.1215</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>TAMPÃO - 1/2 LISO PVC</t>
+          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -8629,20 +8659,20 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>TAMPÃO - 1/2 LISO PVC</t>
+          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
         </is>
       </c>
       <c r="G192" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H192" t="inlineStr">
         <is>
@@ -8658,12 +8688,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>30.26.1156</t>
+          <t>30.26.1215</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Curva 90º para eletroduto PVC rígido, anti-chama, ¾”, fabricante nacional</t>
+          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -8672,7 +8702,7 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -8681,11 +8711,11 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>Curva 90º para eletroduto PVC rígido, anti-chama, ¾”, fabricante nacional</t>
+          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
         </is>
       </c>
       <c r="G193" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="H193" t="inlineStr">
         <is>
@@ -8701,12 +8731,12 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>30.26.1215</t>
+          <t>30.26.1226</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
+          <t>HASTE DE ATERRAMENTO EM COBRE, 5/8" X 2,40M.</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -8715,7 +8745,7 @@
         </is>
       </c>
       <c r="D194" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -8724,15 +8754,15 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
+          <t>HASTE DE ATERRAMENTO EM COBRE, 5/8" X 2,40M.</t>
         </is>
       </c>
       <c r="G194" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
@@ -8744,12 +8774,12 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>30.26.1215</t>
+          <t>30.26.1529</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
+          <t>MULTÍMETRO DIGITAL PORTÁTIL.</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -8758,7 +8788,7 @@
         </is>
       </c>
       <c r="D195" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -8767,15 +8797,15 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>ABRAÇADEIRA PLÁSTICA PARA ELETRODUTO DE 3/4.</t>
+          <t>MULT</t>
         </is>
       </c>
       <c r="G195" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
@@ -8787,12 +8817,12 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>30.26.1226</t>
+          <t>30.26.1646</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>HASTE DE ATERRAMENTO EM COBRE, 5/8" X 2,40M.</t>
+          <t>PARAFUSO, MATERIAL AÇO, 6MM, CABEÇA TIPO PANELA, COM BUCHA 6MM.</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -8801,7 +8831,7 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -8810,11 +8840,11 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>HASTE DE ATERRAMENTO EM COBRE, 5/8" X 2,40M.</t>
+          <t>PARAFUSO, MATERIAL AÇO, 6MM, CABEÇA TIPO PANELA, COM BUCHA 6MM.</t>
         </is>
       </c>
       <c r="G196" t="n">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="H196" t="inlineStr">
         <is>
@@ -8830,12 +8860,12 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>30.26.1529</t>
+          <t>30.26.1975</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>MULTÍMETRO DIGITAL PORTÁTIL.</t>
+          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -8844,7 +8874,7 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -8853,15 +8883,15 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>MULT</t>
+          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
         </is>
       </c>
       <c r="G197" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
@@ -8873,12 +8903,12 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>30.26.1646</t>
+          <t>30.26.1975</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>PARAFUSO, MATERIAL AÇO, 6MM, CABEÇA TIPO PANELA, COM BUCHA 6MM.</t>
+          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -8887,31 +8917,41 @@
         </is>
       </c>
       <c r="D198" t="n">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
           <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
-      <c r="F198" t="inlineStr"/>
-      <c r="G198" t="inlineStr"/>
-      <c r="H198" t="inlineStr"/>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
+        </is>
+      </c>
+      <c r="G198" t="n">
+        <v>3</v>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
+        </is>
+      </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>left_only</t>
+          <t>both</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>30.26.1975</t>
+          <t>30.26.1997</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
+          <t>Lâmpada vapor metálico de 400W.</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -8920,7 +8960,7 @@
         </is>
       </c>
       <c r="D199" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -8929,15 +8969,15 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G199" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I199" t="inlineStr">
@@ -8949,12 +8989,12 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>30.26.1975</t>
+          <t>30.26.2160</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
+          <t>LUVA DE SEGURANÇA, CONFECCIONADA EM RASPA, REFORÇO INTERNO EM RASPA NA PALMA, TIRA DE REFORÇO EXTERNO EM RASPA ENTRE O POLEGAR E O INDICADOR, PROTEÇÃO DAS MÃOS DO USUSARIO CONTRA AGENTES ABRASIVOS E ESCORIANTES, CANO LONGO. MARCA: ZANEL</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -8963,7 +9003,7 @@
         </is>
       </c>
       <c r="D200" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -8972,11 +9012,11 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Caixa de passagem de sobrepor em chapa de aço com entrada para canaleta e eletrodutos 3/4</t>
+          <t>LUVA DE SEGURANÇA, CONFECCIONADA EM RASPA, REFORÇO INTERNO EM RASPA NA PALMA, TIRA DE REFORÇO EXTERNO EM RASPA ENTRE O POLEGAR E O INDICADOR, PROTEÇÃO DAS MÃOS DO USUSARIO CONTRA AGENTES ABRASIVOS E ESCORIANTES, CANO LONGO. MARCA: ZANEL</t>
         </is>
       </c>
       <c r="G200" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H200" t="inlineStr">
         <is>
@@ -8992,21 +9032,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>30.26.1997</t>
+          <t>30.26.2340</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Lâmpada vapor metálico de 400W.</t>
+          <t>CALHA DE ALUMÍNIO, ESTRUTURA SOBREPOR, CAPACIDADE 2 LÂMPADAS FLUORESCENTES E TUBULARES DE ATÉ 40W (PINTURA ELETROSTÁTICA EM PÓ POLIÉSTER)</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -9015,11 +9055,11 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>CALHA DE ALUM</t>
         </is>
       </c>
       <c r="G201" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H201" t="inlineStr">
         <is>
@@ -9035,12 +9075,12 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>30.26.2160</t>
+          <t>30.26.2342</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>LUVA DE SEGURANÇA, CONFECCIONADA EM RASPA, REFORÇO INTERNO EM RASPA NA PALMA, TIRA DE REFORÇO EXTERNO EM RASPA ENTRE O POLEGAR E O INDICADOR, PROTEÇÃO DAS MÃOS DO USUSARIO CONTRA AGENTES ABRASIVOS E ESCORIANTES, CANO LONGO. MARCA: ZANEL</t>
+          <t>LUMINÁRIA DE EMERGÊNCIA AUTÔNOMA, BIVOLT, FLÚOR, 2X10W.</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -9049,7 +9089,7 @@
         </is>
       </c>
       <c r="D202" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -9058,15 +9098,15 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>LUVA DE SEGURANÇA, CONFECCIONADA EM RASPA, REFORÇO INTERNO EM RASPA NA PALMA, TIRA DE REFORÇO EXTERNO EM RASPA ENTRE O POLEGAR E O INDICADOR, PROTEÇÃO DAS MÃOS DO USUSARIO CONTRA AGENTES ABRASIVOS E ESCORIANTES, CANO LONGO. MARCA: ZANEL</t>
+          <t>LUMIN</t>
         </is>
       </c>
       <c r="G202" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I202" t="inlineStr">
@@ -9078,21 +9118,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>30.26.2340</t>
+          <t>30.26.2364</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>CALHA DE ALUMÍNIO, ESTRUTURA SOBREPOR, CAPACIDADE 2 LÂMPADAS FLUORESCENTES E TUBULARES DE ATÉ 40W (PINTURA ELETROSTÁTICA EM PÓ POLIÉSTER)</t>
+          <t>Bota de segurança em couro, com absorção de impacto, palmilha antimicrobiana, fechamento em cadarço, solado em PU, cor preta, nº 39 e 40.</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>PAR</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -9101,11 +9141,11 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>CALHA DE ALUM</t>
+          <t>Bota de seguran</t>
         </is>
       </c>
       <c r="G203" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H203" t="inlineStr">
         <is>
@@ -9121,21 +9161,21 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>30.26.2342</t>
+          <t>30.26.2468</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>LUMINÁRIA DE EMERGÊNCIA AUTÔNOMA, BIVOLT, FLÚOR, 2X10W.</t>
+          <t>SOLDA, TIPO SÓLIDO, DIÂMETRO 1,00 MM APLICAÇÃO SERVIÇOS ELÉTRICO E ELETRÔNICO. ROLO 500 G</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>ROLO</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -9144,11 +9184,11 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>LUMIN</t>
+          <t>SOLDA, TIPO S</t>
         </is>
       </c>
       <c r="G204" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H204" t="inlineStr">
         <is>
@@ -9164,21 +9204,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>30.26.2364</t>
+          <t>30.26.2908</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Bota de segurança em couro, com absorção de impacto, palmilha antimicrobiana, fechamento em cadarço, solado em PU, cor preta, nº 39 e 40.</t>
+          <t>ADAPTADOR, CONEXÃO HDMI MACHO X VGA FÊMEA , CARACTERISTICAS ADCIONAIS RESOLUÇÃO MINIMA: 1080P APLICAÇÃO USO EM VIDEO</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>PAR</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -9187,11 +9227,11 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Bota de seguran</t>
+          <t>ADAPTADOR, CONEX</t>
         </is>
       </c>
       <c r="G205" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H205" t="inlineStr">
         <is>
@@ -9207,12 +9247,12 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>30.26.2468</t>
+          <t>30.26.2911</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>SOLDA, TIPO SÓLIDO, DIÂMETRO 1,00 MM APLICAÇÃO SERVIÇOS ELÉTRICO E ELETRÔNICO. ROLO 500 G</t>
+          <t>CABO EXTENSOR, TIPO FLEXÍVEL, TIPO SAIDA HDMI MACHO X HDMI MACHO 19 PINOS, COMPRIMENTO 15 METROS, APLICAÇÃO MULTIMÍDIA, CARACTERÍSTICAS ADICIONAIS,480I,480P,720P,1080I,1080P</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -9230,7 +9270,7 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>SOLDA, TIPO S</t>
+          <t>CABO EXTENSOR, TIPO FLEX</t>
         </is>
       </c>
       <c r="G206" t="n">
@@ -9250,12 +9290,12 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>30.26.2908</t>
+          <t>30.26.2962</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>ADAPTADOR, CONEXÃO HDMI MACHO X VGA FÊMEA , CARACTERISTICAS ADCIONAIS RESOLUÇÃO MINIMA: 1080P APLICAÇÃO USO EM VIDEO</t>
+          <t>Refletor Solar 100w, com placa solar, acendimento automático, controle remoto.</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -9264,7 +9304,7 @@
         </is>
       </c>
       <c r="D207" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -9273,11 +9313,11 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>ADAPTADOR, CONEX</t>
+          <t>Refletor Solar 100w, com placa solar, acendimento autom</t>
         </is>
       </c>
       <c r="G207" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H207" t="inlineStr">
         <is>
@@ -9293,21 +9333,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>30.26.2911</t>
+          <t>30.26.3129</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>CABO EXTENSOR, TIPO FLEXÍVEL, TIPO SAIDA HDMI MACHO X HDMI MACHO 19 PINOS, COMPRIMENTO 15 METROS, APLICAÇÃO MULTIMÍDIA, CARACTERÍSTICAS ADICIONAIS,480I,480P,720P,1080I,1080P</t>
+          <t>LÂMPADA LED, TENSÃO NOMINAL BIVOLT, POTÊNCIA NOMINAL 15 W, COR BRANCA.</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>ROLO</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -9316,11 +9356,11 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>CABO EXTENSOR, TIPO FLEX</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G208" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H208" t="inlineStr">
         <is>
@@ -9336,12 +9376,12 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>30.26.2962</t>
+          <t>30.26.3130</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Refletor Solar 100w, com placa solar, acendimento automático, controle remoto.</t>
+          <t>LÂMPADA LED, TENSÃO NOMINAL BIVOLT, POTÊNCIA NOMINAL 18 W, TIPO BASE G13, COR BRANCA FRIA.</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -9350,7 +9390,7 @@
         </is>
       </c>
       <c r="D209" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -9359,11 +9399,11 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Refletor Solar 100w, com placa solar, acendimento autom</t>
+          <t>L</t>
         </is>
       </c>
       <c r="G209" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="H209" t="inlineStr">
         <is>
@@ -9379,12 +9419,12 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>30.26.3129</t>
+          <t>30.26.3131</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>LÂMPADA LED, TENSÃO NOMINAL BIVOLT, POTÊNCIA NOMINAL 15 W, COR BRANCA.</t>
+          <t>Refletor, Luminária Led para Poste, potência - 100W / Led: Tipo Cob.</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -9393,7 +9433,7 @@
         </is>
       </c>
       <c r="D210" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -9402,11 +9442,11 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Refletor, Lumin</t>
         </is>
       </c>
       <c r="G210" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H210" t="inlineStr">
         <is>
@@ -9422,12 +9462,12 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>30.26.3130</t>
+          <t>30.26.64</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>LÂMPADA LED, TENSÃO NOMINAL BIVOLT, POTÊNCIA NOMINAL 18 W, TIPO BASE G13, COR BRANCA FRIA.</t>
+          <t>REATOR 400W (LAMPADA VAPOR MERCÚRIO)</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -9436,7 +9476,7 @@
         </is>
       </c>
       <c r="D211" t="n">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -9445,11 +9485,11 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>REATOR 400W (LAMPADA VAPOR MERC</t>
         </is>
       </c>
       <c r="G211" t="n">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="H211" t="inlineStr">
         <is>
@@ -9465,12 +9505,12 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>30.26.3131</t>
+          <t>30.29.46</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Refletor, Luminária Led para Poste, potência - 100W / Led: Tipo Cob.</t>
+          <t>CABO PARA ÁUDIO E VÍDEO, MATERIAL CONDUTOR COBRE, MATERIAL DE ISOLAMENTO CONDUTOR PVC. APLICAÇÃO MICROFONE, ACESSÓRIOS CONECTOR XLR, MATERIAL COBERTURA PVC EMBORRACHADO, 2 M DE COMPRIMENTO. MARCA: SANTO ANGELO.</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -9479,20 +9519,20 @@
         </is>
       </c>
       <c r="D212" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
+          <t>29 - MATERIAL P/ AUDIO, VIDEO E FOTO</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>Refletor, Lumin</t>
+          <t xml:space="preserve">CABO PARA </t>
         </is>
       </c>
       <c r="G212" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="H212" t="inlineStr">
         <is>
@@ -9508,12 +9548,12 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>30.26.64</t>
+          <t>30.29.47</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>REATOR 400W (LAMPADA VAPOR MERCÚRIO)</t>
+          <t>CABO PARA ÁUDIO E VÍDEO, MATERIAL CONDUTOR COBRE, MATERIAL ISOLAMENTO CONDUTOR PVC, APLICAÇÃO MICROFONE, ACESSÓRIOS CONECTOR XLR, MATERIAL COBERTURA PVC EMBORRACHADO, COMPRIMENTO 2 M. MARCA: STARCABLE.</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -9522,20 +9562,20 @@
         </is>
       </c>
       <c r="D213" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
+          <t>29 - MATERIAL P/ AUDIO, VIDEO E FOTO</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>REATOR 400W (LAMPADA VAPOR MERC</t>
+          <t xml:space="preserve">CABO PARA </t>
         </is>
       </c>
       <c r="G213" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H213" t="inlineStr">
         <is>
@@ -9551,12 +9591,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>30.29.46</t>
+          <t>30.42.1052</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>CABO PARA ÁUDIO E VÍDEO, MATERIAL CONDUTOR COBRE, MATERIAL DE ISOLAMENTO CONDUTOR PVC. APLICAÇÃO MICROFONE, ACESSÓRIOS CONECTOR XLR, MATERIAL COBERTURA PVC EMBORRACHADO, 2 M DE COMPRIMENTO. MARCA: SANTO ANGELO.</t>
+          <t>CLAVICULÁRIO, MATERIAL ACRÍLICO, COMPRIMENTO 700 MM, LARGURA 450 MM.</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -9565,20 +9605,20 @@
         </is>
       </c>
       <c r="D214" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>29 - MATERIAL P/ AUDIO, VIDEO E FOTO</t>
+          <t>42 - FERRAMENTAS</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t xml:space="preserve">CABO PARA </t>
+          <t>CLAVICUL</t>
         </is>
       </c>
       <c r="G214" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H214" t="inlineStr">
         <is>
@@ -9594,12 +9634,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>30.29.47</t>
+          <t>30.42.1143</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>CABO PARA ÁUDIO E VÍDEO, MATERIAL CONDUTOR COBRE, MATERIAL ISOLAMENTO CONDUTOR PVC, APLICAÇÃO MICROFONE, ACESSÓRIOS CONECTOR XLR, MATERIAL COBERTURA PVC EMBORRACHADO, COMPRIMENTO 2 M. MARCA: STARCABLE.</t>
+          <t>Broca wídia, material corpo: aço, diâmetro: 10 mm, comprimento: 260 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto.</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -9608,24 +9648,24 @@
         </is>
       </c>
       <c r="D215" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>29 - MATERIAL P/ AUDIO, VIDEO E FOTO</t>
+          <t>42 - FERRAMENTAS</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t xml:space="preserve">CABO PARA </t>
+          <t>Broca wídia, material corpo: aço, diâmetro: 10 mm, comprimento: 260 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto.</t>
         </is>
       </c>
       <c r="G215" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I215" t="inlineStr">
@@ -9637,12 +9677,12 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>30.42.1052</t>
+          <t>30.42.1144</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>CLAVICULÁRIO, MATERIAL ACRÍLICO, COMPRIMENTO 700 MM, LARGURA 450 MM.</t>
+          <t>Broca wídia, material corpo: aço, diâmetro: 12 mm, comprimento: 460 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto .</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -9651,7 +9691,7 @@
         </is>
       </c>
       <c r="D216" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -9660,15 +9700,15 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>CLAVICUL</t>
+          <t>Broca wídia, material corpo: aço, diâmetro: 12 mm, comprimento: 460 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto .</t>
         </is>
       </c>
       <c r="G216" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I216" t="inlineStr">
@@ -9680,12 +9720,12 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>30.42.1143</t>
+          <t>30.42.1145</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Broca wídia, material corpo: aço, diâmetro: 10 mm, comprimento: 260 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto.</t>
+          <t>Broca wídia, material corpo: aço carbono, diâmetro: 8 mm, características adicionais: haste cilíndrica, aplicação: perfuração de concreto .</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -9694,7 +9734,7 @@
         </is>
       </c>
       <c r="D217" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -9703,11 +9743,11 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>Broca wídia, material corpo: aço, diâmetro: 10 mm, comprimento: 260 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto.</t>
+          <t>Broca wídia, material corpo: aço carbono, diâmetro: 8 mm, características adicionais: haste cilíndrica, aplicação: perfuração de concreto .</t>
         </is>
       </c>
       <c r="G217" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H217" t="inlineStr">
         <is>
@@ -9723,21 +9763,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>30.42.1144</t>
+          <t>30.42.1148</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Broca wídia, material corpo: aço, diâmetro: 12 mm, comprimento: 460 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto .</t>
+          <t>FITA ISOLANTE ELÉTRICA, MATERIAL BÁSICO FILME DE PVC, RESISTÊNCIA À TENSÃO ATÉ 750 V, COR PRETA 18mmx20mts.</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>UN</t>
+          <t>ROLO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -9746,15 +9786,15 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>Broca wídia, material corpo: aço, diâmetro: 12 mm, comprimento: 460 mm, características adicionais: encaixe tipo sds plus, aplicação: perfuração de concreto .</t>
+          <t>FITA ISOLANTE EL</t>
         </is>
       </c>
       <c r="G218" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
+          <t>cmpsg@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I218" t="inlineStr">
@@ -9766,12 +9806,12 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>30.42.1145</t>
+          <t>30.42.1149</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Broca wídia, material corpo: aço carbono, diâmetro: 8 mm, características adicionais: haste cilíndrica, aplicação: perfuração de concreto .</t>
+          <t>TORNEIRA, MATERIAL CORPO METAL, TIPO JARDIM, DIÂMETRO 1/2 POL., ACABAMENTO SUPERFICIAL CROMADO, CARACTERÍSTICAS ADICIONAIS ADAPTADOR PARA MANGUEIRA E FECHAMENTO RÁPIDO</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -9780,7 +9820,7 @@
         </is>
       </c>
       <c r="D219" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -9789,11 +9829,11 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>Broca wídia, material corpo: aço carbono, diâmetro: 8 mm, características adicionais: haste cilíndrica, aplicação: perfuração de concreto .</t>
+          <t>TORNEIRA, MATERIAL CORPO METAL, TIPO JARDIM, DIÂMETRO 1/2 POL., ACABAMENTO SUPERFICIAL CROMADO, CARACTERÍSTICAS ADICIONAIS ADAPTADOR PARA MANGUEIRA E FECHAMENTO RÁPIDO</t>
         </is>
       </c>
       <c r="G219" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H219" t="inlineStr">
         <is>
@@ -9809,21 +9849,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>30.42.1148</t>
+          <t>30.42.1151</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>FITA ISOLANTE ELÉTRICA, MATERIAL BÁSICO FILME DE PVC, RESISTÊNCIA À TENSÃO ATÉ 750 V, COR PRETA 18mmx20mts.</t>
+          <t>MANGUEIRA HIDRÁULICA, DIÂMETRO INTERNO 3/4 POL, MATERIAL PVC, COR CRISTAL, TIPO TRANÇADA, ESPESSURA PAREDE 2,4 MM.</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>ROLO</t>
+          <t>METRO</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -9832,11 +9872,11 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>FITA ISOLANTE EL</t>
+          <t>MANGUEIRA HIDR</t>
         </is>
       </c>
       <c r="G220" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="H220" t="inlineStr">
         <is>
@@ -9852,12 +9892,12 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>30.42.1149</t>
+          <t>30.42.1152</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>TORNEIRA, MATERIAL CORPO METAL, TIPO JARDIM, DIÂMETRO 1/2 POL., ACABAMENTO SUPERFICIAL CROMADO, CARACTERÍSTICAS ADICIONAIS ADAPTADOR PARA MANGUEIRA E FECHAMENTO RÁPIDO</t>
+          <t>FITA VEDA ROSCA, MATERIAL TEFLON, COMPRIMENTO 50 M, LARGURA 18 MM.</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -9866,7 +9906,7 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -9875,11 +9915,11 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>TORNEIRA, MATERIAL CORPO METAL, TIPO JARDIM, DIÂMETRO 1/2 POL., ACABAMENTO SUPERFICIAL CROMADO, CARACTERÍSTICAS ADICIONAIS ADAPTADOR PARA MANGUEIRA E FECHAMENTO RÁPIDO</t>
+          <t>FITA VEDA ROSCA, MATERIAL TEFLON, COMPRIMENTO 50 M, LARGURA 18 MM.</t>
         </is>
       </c>
       <c r="G221" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H221" t="inlineStr">
         <is>
@@ -9895,21 +9935,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>30.42.1151</t>
+          <t>30.42.1154</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>MANGUEIRA HIDRÁULICA, DIÂMETRO INTERNO 3/4 POL, MATERIAL PVC, COR CRISTAL, TIPO TRANÇADA, ESPESSURA PAREDE 2,4 MM.</t>
+          <t>TORNEIRA, MATERIAL CORPO LATÃO, TIPO PRESSÃO, DIÂMETRO 1/2 POL, ACABAMENTO CROMADO, APLICAÇÃO LAVATÓRIO - automática</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>METRO</t>
+          <t>UN</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -9918,15 +9958,15 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>MANGUEIRA HIDR</t>
+          <t>TORNEIRA, MATERIAL CORPO LATÃO, TIPO PRESSÃO, DIÂMETRO 1/2 POL, ACABAMENTO CROMADO, APLICAÇÃO LAVATÓRIO - automática</t>
         </is>
       </c>
       <c r="G222" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>cmpsg@jaboatao.ifpe.edu.br</t>
+          <t>ceof@jaboatao.ifpe.edu.br</t>
         </is>
       </c>
       <c r="I222" t="inlineStr">
@@ -9938,12 +9978,12 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>30.42.1152</t>
+          <t>30.42.1155</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>FITA VEDA ROSCA, MATERIAL TEFLON, COMPRIMENTO 50 M, LARGURA 18 MM.</t>
+          <t>FECHADURA, MATERIAL CAIXA AÇO, ACABAMENTO SUPERFICIAL CROMADO, COMPONENTES 2 CHAVES EM LATÃO NIQUELADO, MAÇANETA TIPO ALAVANCA, TIPO INTERNA/EXTERNA, APLICAÇÃO PORTA.</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -9952,7 +9992,7 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -9961,11 +10001,11 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>FITA VEDA ROSCA, MATERIAL TEFLON, COMPRIMENTO 50 M, LARGURA 18 MM.</t>
+          <t>FECHADURA, MATERIAL CAIXA AÇO, ACABAMENTO SUPERFICIAL CROMADO, COMPONENTES 2 CHAVES EM LATÃO NIQUELADO, MAÇANETA TIPO ALAVANCA, TIPO INTERNA/EXTERNA, APLICAÇÃO PORTA.</t>
         </is>
       </c>
       <c r="G223" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H223" t="inlineStr">
         <is>
@@ -9981,12 +10021,12 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>30.42.1154</t>
+          <t>30.42.1160</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>TORNEIRA, MATERIAL CORPO LATÃO, TIPO PRESSÃO, DIÂMETRO 1/2 POL, ACABAMENTO CROMADO, APLICAÇÃO LAVATÓRIO - automática</t>
+          <t>TORNEIRA, Material corpo metal cromado, tipo longa, diâmetro 1/2 pol, acabamento superficial cromado, características adicionais com temporizador, aplicação lavatório - GMC Metais 1093.</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -9995,7 +10035,7 @@
         </is>
       </c>
       <c r="D224" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -10004,11 +10044,11 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>TORNEIRA, MATERIAL CORPO LATÃO, TIPO PRESSÃO, DIÂMETRO 1/2 POL, ACABAMENTO CROMADO, APLICAÇÃO LAVATÓRIO - automática</t>
+          <t>TORNEIRA, Material corpo metal cromado, tipo longa, diâmetro 1/2 pol, acabamento superficial cromado, características adicionais com temporizador, aplicação lavatório - GMC Metais 1093.</t>
         </is>
       </c>
       <c r="G224" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="H224" t="inlineStr">
         <is>
@@ -10024,12 +10064,12 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>30.42.1155</t>
+          <t>30.44.41</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>FECHADURA, MATERIAL CAIXA AÇO, ACABAMENTO SUPERFICIAL CROMADO, COMPONENTES 2 CHAVES EM LATÃO NIQUELADO, MAÇANETA TIPO ALAVANCA, TIPO INTERNA/EXTERNA, APLICAÇÃO PORTA.</t>
+          <t>Círculo ou seta indicativo de H2O. Cor interna: Branca com indicações do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -10038,20 +10078,20 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>42 - FERRAMENTAS</t>
+          <t>44 - MATERIAL DE SINALIZACAO VISUAL E OUTROS</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>FECHADURA, MATERIAL CAIXA AÇO, ACABAMENTO SUPERFICIAL CROMADO, COMPONENTES 2 CHAVES EM LATÃO NIQUELADO, MAÇANETA TIPO ALAVANCA, TIPO INTERNA/EXTERNA, APLICAÇÃO PORTA.</t>
+          <t>Círculo ou seta indicativo de H2O. Cor interna: Branca com indicações do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
         </is>
       </c>
       <c r="G225" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H225" t="inlineStr">
         <is>
@@ -10067,12 +10107,12 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>30.42.1160</t>
+          <t>30.44.42</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>TORNEIRA, Material corpo metal cromado, tipo longa, diâmetro 1/2 pol, acabamento superficial cromado, características adicionais com temporizador, aplicação lavatório - GMC Metais 1093.</t>
+          <t>Círculo ou seta indicativo de CO2. Cor interna: Amarela com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -10081,20 +10121,20 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>42 - FERRAMENTAS</t>
+          <t>44 - MATERIAL DE SINALIZACAO VISUAL E OUTROS</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>TORNEIRA, Material corpo metal cromado, tipo longa, diâmetro 1/2 pol, acabamento superficial cromado, características adicionais com temporizador, aplicação lavatório - GMC Metais 1093.</t>
+          <t>Círculo ou seta indicativo de CO2. Cor interna: Amarela com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
         </is>
       </c>
       <c r="G226" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="H226" t="inlineStr">
         <is>
@@ -10110,12 +10150,12 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>30.44.41</t>
+          <t>30.44.43</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Círculo ou seta indicativo de H2O. Cor interna: Branca com indicações do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
+          <t>Círculo ou seta indicativo de PQS. Cor interna: Azul com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -10124,7 +10164,7 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -10133,11 +10173,11 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>Círculo ou seta indicativo de H2O. Cor interna: Branca com indicações do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
+          <t>Círculo ou seta indicativo de PQS. Cor interna: Azul com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha</t>
         </is>
       </c>
       <c r="G227" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H227" t="inlineStr">
         <is>
@@ -10153,12 +10193,12 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>30.44.42</t>
+          <t>30.44.60</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Círculo ou seta indicativo de CO2. Cor interna: Amarela com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
+          <t>PLACA SINALIZADORA DE SAIDA DE EMERGENCIA, COM FUNDO VERDE E SETA DIRECIONAL.</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -10167,7 +10207,7 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -10176,11 +10216,11 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Círculo ou seta indicativo de CO2. Cor interna: Amarela com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha.</t>
+          <t>PLACA SINALIZADORA DE SAIDA DE EMERGENCIA, COM FUNDO VERDE E SETA DIRECIONAL.</t>
         </is>
       </c>
       <c r="G228" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H228" t="inlineStr">
         <is>
@@ -10188,92 +10228,6 @@
         </is>
       </c>
       <c r="I228" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>30.44.43</t>
-        </is>
-      </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>Círculo ou seta indicativo de PQS. Cor interna: Azul com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha</t>
-        </is>
-      </c>
-      <c r="C229" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="D229" t="n">
-        <v>2</v>
-      </c>
-      <c r="E229" t="inlineStr">
-        <is>
-          <t>44 - MATERIAL DE SINALIZACAO VISUAL E OUTROS</t>
-        </is>
-      </c>
-      <c r="F229" t="inlineStr">
-        <is>
-          <t>Círculo ou seta indicativo de PQS. Cor interna: Azul com indicação do fone do Corpo de Bombeiros e cor externa: Vermelha</t>
-        </is>
-      </c>
-      <c r="G229" t="n">
-        <v>2</v>
-      </c>
-      <c r="H229" t="inlineStr">
-        <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
-        </is>
-      </c>
-      <c r="I229" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>30.44.60</t>
-        </is>
-      </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>PLACA SINALIZADORA DE SAIDA DE EMERGENCIA, COM FUNDO VERDE E SETA DIRECIONAL.</t>
-        </is>
-      </c>
-      <c r="C230" t="inlineStr">
-        <is>
-          <t>UN</t>
-        </is>
-      </c>
-      <c r="D230" t="n">
-        <v>30</v>
-      </c>
-      <c r="E230" t="inlineStr">
-        <is>
-          <t>44 - MATERIAL DE SINALIZACAO VISUAL E OUTROS</t>
-        </is>
-      </c>
-      <c r="F230" t="inlineStr">
-        <is>
-          <t>PLACA SINALIZADORA DE SAIDA DE EMERGENCIA, COM FUNDO VERDE E SETA DIRECIONAL.</t>
-        </is>
-      </c>
-      <c r="G230" t="n">
-        <v>30</v>
-      </c>
-      <c r="H230" t="inlineStr">
-        <is>
-          <t>ceof@jaboatao.ifpe.edu.br</t>
-        </is>
-      </c>
-      <c r="I230" t="inlineStr">
         <is>
           <t>both</t>
         </is>

</xml_diff>